<commit_message>
added bulk of explanations
</commit_message>
<xml_diff>
--- a/dog snps.xlsx
+++ b/dog snps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliajones/Desktop/FA21/BIMM143/LCORL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C626D8-EFBA-0D43-9154-9F0811DC4043}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51859837-F593-B54E-B6B5-0C7B38CC0545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9820" yWindow="500" windowWidth="18980" windowHeight="16400" activeTab="1" xr2:uid="{6446846C-F3F8-A84A-961B-A682F56D7684}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="75">
   <si>
     <t>igf1</t>
   </si>
@@ -961,10 +961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBEDD088-87D2-CC46-807C-4EFA9FA05D81}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -984,44 +984,52 @@
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>74</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>